<commit_message>
Ajustes Informes de OT
</commit_message>
<xml_diff>
--- a/downloads/informeAvanceOT.xlsx
+++ b/downloads/informeAvanceOT.xlsx
@@ -130,7 +130,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -158,44 +158,24 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tipo</t>
+          <t>frente</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>cantidad</t>
+          <t>planeado_frente</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>duracion</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>frente</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>tarifa</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>cant_planeada</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>ejecuccion</t>
+          <t>ejecutado</t>
         </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>TEST</t>
         </is>
       </c>
       <c r="B2" s="0" t="n">
@@ -208,38 +188,20 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>actividad</t>
-        </is>
-      </c>
-      <c r="E2" s="0" t="inlineStr">
-        <is>
-          <t>0.1</t>
-        </is>
+          <t>frente 1 - TEST 1</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1.03</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="0" t="inlineStr">
-        <is>
-          <t>frente 2 test2</t>
-        </is>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>247306</v>
-      </c>
-      <c r="I2" s="0" t="inlineStr">
-        <is>
-          <t>0.1</t>
-        </is>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>4.00000</v>
+        <v>5.00000</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>TEST</t>
         </is>
       </c>
       <c r="B3" s="0" t="n">
@@ -252,32 +214,118 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>actividad</t>
-        </is>
-      </c>
-      <c r="E3" s="0" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
+          <t>frente 1 - TEST 1</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="0" t="inlineStr">
-        <is>
-          <t>frente 1 test1</t>
-        </is>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>321344</v>
-      </c>
-      <c r="I3" s="0" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>4.00000</v>
+        <v>6.00000</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>10103</v>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>EXCAVACIÓN MANUAL BAJO AGUA PARA LABORES CONVENCIONALES</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>frente 1 - TEST 1</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>7.00000</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>10101</v>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>EXCAVACIÓN MANUAL EN TIERRA PARA LABORES CONVENCIONALES</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>frente 2 - TEST 2</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>3.00000</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>10102</v>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>EXCAVACIÓN MANUAL EN CONGLOMERADO PARA LABORES CONVENCIONALES</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>frente 2 - TEST 2</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.00000</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>10103</v>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>EXCAVACIÓN MANUAL BAJO AGUA PARA LABORES CONVENCIONALES</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>frente 2 - TEST 2</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>3.00000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>